<commit_message>
-mapeo estaciones creado en qlik -readme visualizaciones -algunos ejemplos visuales -algun cambio menor y eliminados algunos warnings en los jupyters de meteo
</commit_message>
<xml_diff>
--- a/visualizaciones qlik/Geo_puntos_AQI/geopoints_csv_aqi.xlsx
+++ b/visualizaciones qlik/Geo_puntos_AQI/geopoints_csv_aqi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaume\Documents\0.CURSO BIG DATA.MIRADAX TELEFONICA\Proyectos repositorios git\ProyectoBigData\visualizaciones qlik\Geo_puntos_AQI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaume\Documents\0.Curso Big Data\0GIT.Proyectos\ProyectoBigData\visualizaciones qlik\Geo_puntos_AQI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989FDEB-2965-4C73-9A84-1AD04BA5B3CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332AC107-E9C1-46B6-9FD6-3B0F8DCD3F35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{C3F4D5B9-7F9B-4E8C-8FAC-7040551F9A42}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{C3F4D5B9-7F9B-4E8C-8FAC-7040551F9A42}"/>
   </bookViews>
   <sheets>
     <sheet name="geo_aqi_points" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="88">
   <si>
     <t>Ciudad</t>
   </si>
@@ -105,9 +105,6 @@
     <t>barcelona</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Distrito+del+Ensanche,+Barcelona/@41.3934752,2.1296575,13z/data=!3m1!4b1!4m5!3m4!1s0x12a4a28d7b963ea1:0x9ee6d50544f5205d!8m2!3d41.3922186!4d2.164864</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/search/barcelona-(gr%C3%A0cia-st.gervasi)/@41.3934646,2.1296575,13z/data=!3m1!4b1</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>https://www.google.com/maps/search/fernandez-ladreda,+madrid/@40.3851266,-3.7258962,15z/data=!3m1!4b1</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/place/Madrid/@40.4376161,-3.9597143,10z/data=!3m1!4b1!4m5!3m4!1s0xd422997800a3c81:0xc436dec1618c2269!8m2!3d40.4167754!4d-3.7037902</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/place/C.+de+M%C3%A9ndez+%C3%81lvaro,+Madrid/@40.3988882,-3.6925589,15z/data=!3m1!4b1!4m5!3m4!1s0xd42263dffc6d6a9:0x72828c40751d45cb!8m2!3d40.3988885!4d-3.6838041</t>
   </si>
   <si>
@@ -153,102 +147,9 @@
     <t>https://www.google.com/maps/search/barcelona-(palau+reial)/@41.4294412,2.0760718,12z/data=!3m1!4b1</t>
   </si>
   <si>
-    <t>2.1296575</t>
-  </si>
-  <si>
-    <t>2.0760718</t>
-  </si>
-  <si>
-    <t>2.1286017</t>
-  </si>
-  <si>
-    <t>2.184758</t>
-  </si>
-  <si>
-    <t>2.0086857</t>
-  </si>
-  <si>
-    <t>2.0427628</t>
-  </si>
-  <si>
-    <t>2.1866325</t>
-  </si>
-  <si>
     <t>url.gmaps</t>
   </si>
   <si>
-    <t>-3.8181148</t>
-  </si>
-  <si>
-    <t>-3.6935587</t>
-  </si>
-  <si>
-    <t>-3.7145547</t>
-  </si>
-  <si>
-    <t>-3.6903721</t>
-  </si>
-  <si>
-    <t>-3.7258962</t>
-  </si>
-  <si>
-    <t>-3.9597143</t>
-  </si>
-  <si>
-    <t>-3.6925589</t>
-  </si>
-  <si>
-    <t>-3.6986151</t>
-  </si>
-  <si>
-    <t>41.3934752</t>
-  </si>
-  <si>
-    <t>41.3934646</t>
-  </si>
-  <si>
-    <t>41.4294412</t>
-  </si>
-  <si>
-    <t>41.4294637</t>
-  </si>
-  <si>
-    <t>41.3995657</t>
-  </si>
-  <si>
-    <t>41.3947051</t>
-  </si>
-  <si>
-    <t>41.3617218</t>
-  </si>
-  <si>
-    <t>41.4238926</t>
-  </si>
-  <si>
-    <t>40.4242288</t>
-  </si>
-  <si>
-    <t>40.4334632</t>
-  </si>
-  <si>
-    <t>40.4518651</t>
-  </si>
-  <si>
-    <t>40.4216356</t>
-  </si>
-  <si>
-    <t>40.3851266</t>
-  </si>
-  <si>
-    <t>40.4376161</t>
-  </si>
-  <si>
-    <t>40.3988882</t>
-  </si>
-  <si>
-    <t>40.4658568</t>
-  </si>
-  <si>
     <t>barcelona-(eixample), catalunya, spain-air-quality.csv</t>
   </si>
   <si>
@@ -295,6 +196,108 @@
   </si>
   <si>
     <t>plaza-de castilla, madrid-air-quality.csv</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Distrito+del+Ensanche,+Barcelona/@41.3934752,2.1296574,13z/data=!3m1!4b1!4m5!3m4!1s0x12a4a28d7b963ea1:0x9ee6d50544f5205d!8m2!3d41.3922186!4d2.164864</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps/place/Madrid/@40.4378698,-3.8196207,11z/data=!3m1!4b1!4m5!3m4!1s0xd422997800a3c81:0xc436dec1618c2269!8m2!3d40.4167754!4d-3.7037902</t>
+  </si>
+  <si>
+    <t>40.42022989632735</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -3.703493697910503</t>
+  </si>
+  <si>
+    <t>-3.6837826444763206</t>
+  </si>
+  <si>
+    <t>40.39904371972173</t>
+  </si>
+  <si>
+    <t>-3.6898817598165854</t>
+  </si>
+  <si>
+    <t>40.466020327591245</t>
+  </si>
+  <si>
+    <t>-3.7172808770103365</t>
+  </si>
+  <si>
+    <t>40.385314840264606</t>
+  </si>
+  <si>
+    <t>-3.681638759817924</t>
+  </si>
+  <si>
+    <t>40.42171755724618</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -3.7024525162685133</t>
+  </si>
+  <si>
+    <t>40.451441584114214</t>
+  </si>
+  <si>
+    <t>-3.687121361634064</t>
+  </si>
+  <si>
+    <t>40.43545573137402</t>
+  </si>
+  <si>
+    <t>-3.748419198004095</t>
+  </si>
+  <si>
+    <t>40.41940934731714</t>
+  </si>
+  <si>
+    <t>2.224741624843516</t>
+  </si>
+  <si>
+    <t>41.42750061932972</t>
+  </si>
+  <si>
+    <t>2.1162349595930863</t>
+  </si>
+  <si>
+    <t>41.368308245126215</t>
+  </si>
+  <si>
+    <t>2.1659319226470184</t>
+  </si>
+  <si>
+    <t>41.398116890348625</t>
+  </si>
+  <si>
+    <t>2.2027825514365285</t>
+  </si>
+  <si>
+    <t>41.40352610070857</t>
+  </si>
+  <si>
+    <t>2.141085038363847</t>
+  </si>
+  <si>
+    <t>41.42161323412011</t>
+  </si>
+  <si>
+    <t>2.1773519002395694</t>
+  </si>
+  <si>
+    <t>41.38845704993374</t>
+  </si>
+  <si>
+    <t>2.1420170916729235</t>
+  </si>
+  <si>
+    <t>41.40362665375243</t>
+  </si>
+  <si>
+    <t>2.164504621095891</t>
+  </si>
+  <si>
+    <t>41.39128592807325</t>
   </si>
 </sst>
 </file>
@@ -318,12 +321,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -342,8 +351,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -662,7 +671,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +701,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -700,19 +709,19 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,19 +729,19 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,19 +749,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -760,19 +769,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -780,19 +789,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -800,19 +809,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -820,19 +829,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,19 +849,19 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -860,19 +869,19 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -880,19 +889,19 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -900,19 +909,19 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,19 +929,19 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -940,19 +949,19 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -960,19 +969,19 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,19 +989,19 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1000,19 +1009,19 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>